<commit_message>
n320: Add support for Rev B Rhodium
- Updated JESD core files, removing MGT refclk export to fabric.
- Updated RadioClocking to no longer use MGT refclk for the MMCM.
- Updated DbCore with the new JESD core and RadioClocking module.
- Updated and cleaned up FPGA pinout.
- Updated FPGA timing constraints.
- Updated top-level FPGA for new JESD core.
- Placed SYSREF sampling FFs in IOBs.
</commit_message>
<xml_diff>
--- a/usrp3/top/n3xx/dboards/rh/doc/rh_timing.xlsx
+++ b/usrp3/top/n3xx/dboards/rh/doc/rh_timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\fpgadev\usrp3\top\n3xx\dboards\rh\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC4BD6C-CB6B-4AA2-8B7D-C9F62ABEB08F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3395A64D-EF75-44FB-BF19-0B8EDFE16AFE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SYSREF Transmit (not used)" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22,12 +22,12 @@
     <sheet name="PS SPI at CPLD" sheetId="7" r:id="rId7"/>
     <sheet name="PS SPI at FPGA" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="191">
   <si>
     <t>SPI timing through the CPLD for passthrough interfaces</t>
   </si>
@@ -589,6 +589,18 @@
   <si>
     <t>* The cell highlighted in yellow is the overconstrained read-only frequency.</t>
   </si>
+  <si>
+    <t>worst case for n320</t>
+  </si>
+  <si>
+    <t>There are actually 2 constraints needed: DBA / LMK DBB / LMK</t>
+  </si>
+  <si>
+    <t>* Positive leg of diff pair used.</t>
+  </si>
+  <si>
+    <t>datasheet * 10 (arbitrary)</t>
+  </si>
 </sst>
 </file>
 
@@ -913,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -992,6 +1004,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1403,15 +1417,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1432,7 +1446,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="5295900" y="3457575"/>
           <a:ext cx="5638800" cy="2743200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2089,19 +2103,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -2187,10 +2201,10 @@
         <f t="shared" si="1"/>
         <v>0.69513000000000014</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="64"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -2349,12 +2363,12 @@
       <c r="A11" s="2"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
@@ -2594,12 +2608,12 @@
       <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
@@ -5750,19 +5764,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="66"/>
       <c r="J1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -5851,10 +5865,10 @@
         <f t="shared" si="1"/>
         <v>0.22695000000000001</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="64"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -5891,11 +5905,11 @@
       <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="F6" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="H6" s="64"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="66"/>
       <c r="K6" s="3" t="s">
         <v>27</v>
       </c>
@@ -5991,12 +6005,12 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6179,12 +6193,12 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
@@ -9242,11 +9256,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:X987"/>
+  <dimension ref="A1:AA987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9256,32 +9270,34 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="13" max="13" width="84.7109375" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="60" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="16" max="16" width="84.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="2"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -9291,8 +9307,11 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -9303,17 +9322,26 @@
         <v>6</v>
       </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -9326,54 +9354,74 @@
       <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="10">
-        <f>121+1091+2877</f>
-        <v>4089</v>
-      </c>
-      <c r="H3" s="8">
-        <f t="shared" ref="H3:H6" si="0">G3/1000*$B$2</f>
-        <v>0.65424000000000004</v>
-      </c>
-      <c r="I3" s="8">
-        <f t="shared" ref="I3:I6" si="1">G3/1000*$B$3</f>
-        <v>0.69513000000000014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="61">
+        <v>1318.39</v>
+      </c>
+      <c r="H3" s="61">
+        <v>2810.2</v>
+      </c>
+      <c r="I3" s="10">
+        <f>G3+H3</f>
+        <v>4128.59</v>
+      </c>
+      <c r="J3" s="42">
+        <f>0.5*$B$3</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K3" s="8">
+        <f>I3/1000*$B$2</f>
+        <v>0.66057440000000001</v>
+      </c>
+      <c r="L3" s="8">
+        <f>I3/1000*$B$3+J3</f>
+        <v>0.78686029999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="9">
-        <f>1/153600000*1000000000</f>
-        <v>6.510416666666667</v>
+        <f>1/250000000*1000000000</f>
+        <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>187</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="10">
-        <f>121+1091+3293</f>
-        <v>4505</v>
-      </c>
-      <c r="H4" s="8">
-        <f t="shared" si="0"/>
-        <v>0.7208</v>
-      </c>
-      <c r="I4" s="8">
-        <f t="shared" si="1"/>
-        <v>0.76585000000000003</v>
-      </c>
-      <c r="K4" s="62" t="s">
+      <c r="G4" s="61">
+        <v>1318.39</v>
+      </c>
+      <c r="H4" s="61">
+        <v>3252.2</v>
+      </c>
+      <c r="I4" s="10">
+        <f t="shared" ref="I4:I6" si="0">G4+H4</f>
+        <v>4570.59</v>
+      </c>
+      <c r="J4" s="42">
+        <f>0.5*$B$3</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" ref="K4:K6" si="1">I4/1000*$B$2</f>
+        <v>0.73129440000000001</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" ref="L4:L6" si="2">I4/1000*$B$3+J4</f>
+        <v>0.86200030000000005</v>
+      </c>
+      <c r="N4" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="64"/>
-    </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O4" s="66"/>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -9389,36 +9437,46 @@
       <c r="F5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="10">
-        <f>1030+2971</f>
-        <v>4001</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="G5" s="61">
+        <v>1848.95</v>
+      </c>
+      <c r="H5" s="61">
+        <v>2987.4</v>
+      </c>
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
-        <v>0.64016000000000006</v>
-      </c>
-      <c r="I5" s="8">
+        <v>4836.3500000000004</v>
+      </c>
+      <c r="J5" s="42">
+        <f t="shared" ref="J5:J6" si="3">0.5*$B$3</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K5" s="8">
         <f t="shared" si="1"/>
-        <v>0.68017000000000005</v>
-      </c>
-      <c r="K5" s="3" t="s">
+        <v>0.77381600000000006</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="2"/>
+        <v>0.90717950000000014</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="18">
+      <c r="O5" s="18">
         <f>B6-C25</f>
-        <v>0.64593000000000078</v>
-      </c>
-      <c r="M5" s="1" t="s">
+        <v>0.66087010000000035</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="9">
         <f>B4</f>
-        <v>6.510416666666667</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
@@ -9429,27 +9487,37 @@
       <c r="F6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="10">
-        <f>1030+2049</f>
-        <v>3079</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="G6" s="61">
+        <v>1848.95</v>
+      </c>
+      <c r="H6" s="61">
+        <v>3541.9</v>
+      </c>
+      <c r="I6" s="10">
         <f t="shared" si="0"/>
-        <v>0.49264000000000002</v>
-      </c>
-      <c r="I6" s="8">
+        <v>5390.85</v>
+      </c>
+      <c r="J6" s="42">
+        <f t="shared" si="3"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K6" s="8">
         <f t="shared" si="1"/>
-        <v>0.52343000000000006</v>
-      </c>
-      <c r="K6" s="3" t="s">
+        <v>0.86253600000000008</v>
+      </c>
+      <c r="L6" s="8">
+        <f t="shared" si="2"/>
+        <v>1.0014445000000001</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="18">
+      <c r="O6" s="18">
         <f>C39</f>
-        <v>-0.90569</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>-0.47946429999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -9462,43 +9530,49 @@
       <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="G7" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="9">
+      <c r="O7" s="9">
         <f>C25</f>
-        <v>5.8644866666666662</v>
-      </c>
-      <c r="M7" s="1" t="s">
+        <v>3.3391298999999997</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="11">
-        <f>0.025*20</f>
-        <v>0.5</v>
+        <f>0.025*8</f>
+        <v>0.2</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L8" s="9">
+      <c r="O8" s="9">
         <f>C39</f>
-        <v>-0.90569</v>
-      </c>
-      <c r="M8" s="1" t="s">
+        <v>-0.47946429999999995</v>
+      </c>
+      <c r="P8" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>75</v>
       </c>
@@ -9513,7 +9587,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -9528,21 +9602,23 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="F13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>44</v>
       </c>
@@ -9558,18 +9634,20 @@
       <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="17">
         <f>B7+B8</f>
-        <v>0.42</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="C15" s="19">
         <f>B15</f>
-        <v>0.42</v>
+        <v>0.12000000000000001</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>57</v>
@@ -9577,8 +9655,10 @@
       <c r="F15" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -9587,50 +9667,54 @@
         <v>0</v>
       </c>
       <c r="C16" s="19">
-        <f t="shared" ref="C16:C17" si="2">C15+B16</f>
-        <v>0.42</v>
+        <f t="shared" ref="C16:C17" si="4">C15+B16</f>
+        <v>0.12000000000000001</v>
       </c>
       <c r="D16" s="1"/>
       <c r="F16" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="19">
-        <f>MAX(I5:I6)</f>
-        <v>0.68017000000000005</v>
+        <f>MAX(L5:L6)</f>
+        <v>1.0014445000000001</v>
       </c>
       <c r="C17" s="19">
-        <f t="shared" si="2"/>
-        <v>1.1001700000000001</v>
+        <f t="shared" si="4"/>
+        <v>1.1214445000000002</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="23">
         <f>C17</f>
-        <v>1.1001700000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.1214445000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="F19" s="41" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>76</v>
       </c>
@@ -9644,34 +9728,34 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="17">
         <f>B6</f>
-        <v>6.510416666666667</v>
+        <v>4</v>
       </c>
       <c r="C21" s="19">
         <f>B21</f>
-        <v>6.510416666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="19">
-        <f>MIN(H3:H4)</f>
-        <v>0.65424000000000004</v>
+        <f>MIN(K3:K4)</f>
+        <v>0.66057440000000001</v>
       </c>
       <c r="C22" s="19">
-        <f t="shared" ref="C22:C23" si="3">C21+B22</f>
-        <v>7.1646566666666667</v>
+        <f t="shared" ref="C22:C23" si="5">C21+B22</f>
+        <v>4.6605743999999998</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>82</v>
       </c>
@@ -9680,45 +9764,45 @@
         <v>-0.2</v>
       </c>
       <c r="C23" s="19">
-        <f t="shared" si="3"/>
-        <v>6.9646566666666665</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="5"/>
+        <v>4.4605743999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
         <v>85</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="23">
         <f>C23</f>
-        <v>6.9646566666666665</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4.4605743999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="23">
         <f>C24-C18</f>
-        <v>5.8644866666666662</v>
+        <v>3.3391298999999997</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="65" t="s">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
         <v>90</v>
       </c>
@@ -9732,24 +9816,26 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="17">
         <f>B7+-B8</f>
-        <v>-0.57999999999999996</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="C29" s="19">
         <f>B29</f>
-        <v>-0.57999999999999996</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
@@ -9758,35 +9844,35 @@
         <v>0</v>
       </c>
       <c r="C30" s="19">
-        <f t="shared" ref="C30:C31" si="4">C29+B30</f>
-        <v>-0.57999999999999996</v>
+        <f t="shared" ref="C30:C31" si="6">C29+B30</f>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B31" s="19">
-        <f>MAX(H5:H6)</f>
-        <v>0.64016000000000006</v>
+        <f>MAX(K5:K6)</f>
+        <v>0.86253600000000008</v>
       </c>
       <c r="C31" s="19">
-        <f t="shared" si="4"/>
-        <v>6.0160000000000102E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.58253600000000005</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="23">
         <f>C31</f>
-        <v>6.0160000000000102E-2</v>
+        <v>0.58253600000000005</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9826,12 +9912,12 @@
         <v>65</v>
       </c>
       <c r="B36" s="19">
-        <f>MAX(I3:I4)</f>
-        <v>0.76585000000000003</v>
+        <f>MAX(L3:L4)</f>
+        <v>0.86200030000000005</v>
       </c>
       <c r="C36" s="19">
-        <f t="shared" ref="C36:C37" si="5">C35+B36</f>
-        <v>0.76585000000000003</v>
+        <f t="shared" ref="C36:C37" si="7">C35+B36</f>
+        <v>0.86200030000000005</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -9844,8 +9930,8 @@
         <v>0.2</v>
       </c>
       <c r="C37" s="19">
-        <f t="shared" si="5"/>
-        <v>0.9658500000000001</v>
+        <f t="shared" si="7"/>
+        <v>1.0620003</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9855,7 +9941,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="23">
         <f>C37</f>
-        <v>0.9658500000000001</v>
+        <v>1.0620003</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9865,7 +9951,7 @@
       <c r="B39" s="25"/>
       <c r="C39" s="23">
         <f>C32-C38</f>
-        <v>-0.90569</v>
+        <v>-0.47946429999999995</v>
       </c>
       <c r="D39" s="26" t="s">
         <v>103</v>
@@ -12718,9 +12804,9 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F1:L1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
     <mergeCell ref="A27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="C25 C39">
@@ -12733,28 +12819,29 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="O7">
     <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7">
+  <conditionalFormatting sqref="O7">
     <cfRule type="cellIs" dxfId="30" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="O8">
     <cfRule type="cellIs" dxfId="29" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8">
+  <conditionalFormatting sqref="O8">
     <cfRule type="cellIs" dxfId="28" priority="6" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12764,7 +12851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12786,22 +12873,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -12911,21 +12998,21 @@
         <v>5323.8559999999998</v>
       </c>
       <c r="J4" s="42">
-        <f t="shared" ref="J4:J6" si="1">0.5*$B$3</f>
+        <f>0.5*$B$3</f>
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="K4" s="8">
-        <f t="shared" ref="K4:K6" si="2">I4/1000*$B$2</f>
+        <f t="shared" ref="K4:K6" si="1">I4/1000*$B$2</f>
         <v>0.85181696000000007</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" ref="L4:L6" si="3">I4/1000*$B$3+J4</f>
+        <f t="shared" ref="L4:L6" si="2">I4/1000*$B$3+J4</f>
         <v>0.99005552000000008</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="70"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -12955,15 +13042,15 @@
         <v>5948.9940000000006</v>
       </c>
       <c r="J5" s="42">
+        <f t="shared" ref="J5:J6" si="3">0.5*$B$3</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K5" s="8">
         <f t="shared" si="1"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="K5" s="8">
+        <v>0.95183904000000019</v>
+      </c>
+      <c r="L5" s="8">
         <f t="shared" si="2"/>
-        <v>0.95183904000000019</v>
-      </c>
-      <c r="L5" s="8">
-        <f t="shared" si="3"/>
         <v>1.0963289800000002</v>
       </c>
       <c r="N5" s="28" t="s">
@@ -13005,15 +13092,15 @@
         <v>5477.8559999999998</v>
       </c>
       <c r="J6" s="42">
+        <f t="shared" si="3"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K6" s="8">
         <f t="shared" si="1"/>
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="K6" s="8">
+        <v>0.87645696000000006</v>
+      </c>
+      <c r="L6" s="8">
         <f t="shared" si="2"/>
-        <v>0.87645696000000006</v>
-      </c>
-      <c r="L6" s="8">
-        <f t="shared" si="3"/>
         <v>1.0162355200000002</v>
       </c>
       <c r="N6" s="28" t="s">
@@ -13109,12 +13196,12 @@
       <c r="A11" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -13283,12 +13370,12 @@
       <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
@@ -16333,7 +16420,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16358,22 +16445,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -16494,17 +16581,17 @@
         <v>0.85181696000000007</v>
       </c>
       <c r="L4" s="8">
-        <f t="shared" si="0"/>
+        <f>I4/1000*$B$3</f>
         <v>0.90505552000000011</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="O4" s="68"/>
-      <c r="Q4" s="67" t="s">
+      <c r="O4" s="70"/>
+      <c r="Q4" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="R4" s="68"/>
+      <c r="R4" s="70"/>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -16722,12 +16809,12 @@
       <c r="A12" s="2"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
       <c r="H14" s="41"/>
@@ -16952,12 +17039,12 @@
       <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
@@ -20057,7 +20144,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20079,22 +20166,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -20215,10 +20302,10 @@
         <f t="shared" ref="L4:L6" si="3">I4/1000*$B$3+J4</f>
         <v>1.4233992900000001</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="70"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -20434,12 +20521,12 @@
       <c r="A12" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -20642,12 +20729,12 @@
       <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
@@ -23723,7 +23810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AA992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -23747,22 +23834,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -23883,10 +23970,10 @@
         <f t="shared" ref="L4:L6" si="2">I4/1000*$B$3+J4</f>
         <v>1.4233992900000001</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="70"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -24027,11 +24114,11 @@
       <c r="D8" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="G8" s="63"/>
-      <c r="H8" s="64"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="66"/>
       <c r="I8" s="48"/>
       <c r="J8" s="48"/>
       <c r="K8" s="48"/>
@@ -24117,12 +24204,12 @@
       <c r="A12" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -24367,12 +24454,12 @@
       <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">

</xml_diff>